<commit_message>
adding test cases outputs
</commit_message>
<xml_diff>
--- a/Grades Sheet Model/output.xlsx
+++ b/Grades Sheet Model/output.xlsx
@@ -453,8 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180236
-</t>
+          <t>31986</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -470,8 +469,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180333
-</t>
+          <t>113333</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -487,8 +485,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180128
-</t>
+          <t>1111768</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -504,8 +501,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180255,
-</t>
+          <t>10865</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -513,14 +509,13 @@
       </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180274
-</t>
+          <t>11274</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -536,8 +531,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180056
-</t>
+          <t>0566</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -551,8 +545,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180041
-</t>
+          <t>01801</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -568,8 +561,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180606,
-</t>
+          <t>18000600</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -582,20 +574,18 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180456
-</t>
+          <t>80056</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">2200022
-</t>
+          <t>20027</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -611,8 +601,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180552
-</t>
+          <t>101552</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,15 +611,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180207
-</t>
+          <t>11207</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
         <v>5</v>
@@ -639,8 +627,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180045
-</t>
+          <t>10005</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -656,8 +643,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180212
-</t>
+          <t>812</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -667,14 +653,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180155
-</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -688,8 +673,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">1170343
-</t>
+          <t>17023</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,8 +686,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">1180172
-</t>
+          <t>8101172</t>
         </is>
       </c>
       <c r="B18" t="n">

</xml_diff>